<commit_message>
fill in Test Report, update SRS with contributions
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD4DFA5-42F4-42FC-9B6F-7578E252B060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -83,26 +86,217 @@
     <t>Low Impact</t>
   </si>
   <si>
-    <t>Test that the water heater is activated if the water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>Water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>From the LCD main menu, select the option "Black Coffee"</t>
-  </si>
-  <si>
-    <t>-Heating element is activated when water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
     <t>REQ-06</t>
+  </si>
+  <si>
+    <t>REQ-01</t>
+  </si>
+  <si>
+    <t>REQ-02</t>
+  </si>
+  <si>
+    <t>REQ-03</t>
+  </si>
+  <si>
+    <t>REQ-04</t>
+  </si>
+  <si>
+    <t>REQ-05</t>
+  </si>
+  <si>
+    <t>REQ-07</t>
+  </si>
+  <si>
+    <t>REQ-08</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>REQ-18</t>
+  </si>
+  <si>
+    <t>REQ-23</t>
+  </si>
+  <si>
+    <t>Webserver Container is running (SPmartWeb)</t>
+  </si>
+  <si>
+    <t>Open Localhost/IP Adderess of RPI</t>
+  </si>
+  <si>
+    <t>Products can be seen and added to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that Web Server page shortcuts are shown correctly </t>
+  </si>
+  <si>
+    <t>Test that Web Server pages are shown correctly and content is shown (products)</t>
+  </si>
+  <si>
+    <t>Webserver Container is running (SPmartWeb) Products are added to cart and user is logged in</t>
+  </si>
+  <si>
+    <t>Shortcuts can be seen in Navbar</t>
+  </si>
+  <si>
+    <t>Add a product to cart</t>
+  </si>
+  <si>
+    <t>Test that cart pages functions properly</t>
+  </si>
+  <si>
+    <t>Products are shown in cart and checkout options are shown</t>
+  </si>
+  <si>
+    <t>Test that checkout options works properly</t>
+  </si>
+  <si>
+    <t>Choose a checkout option and checkout</t>
+  </si>
+  <si>
+    <t>Additional price for delivery is shown and added if selected. When checkout, sent to My Orders</t>
+  </si>
+  <si>
+    <t>Test that orders are shown and Self Pickup QR codes are shown</t>
+  </si>
+  <si>
+    <t>Webserver Container is running (SPmartWeb). Order is placed and user is logged in</t>
+  </si>
+  <si>
+    <t>Checkout/Go to My Orders page</t>
+  </si>
+  <si>
+    <t>Orders are shown and QR codes shown where applicable</t>
+  </si>
+  <si>
+    <t>Test that LCD shows menu as required</t>
+  </si>
+  <si>
+    <t>Python Container is running (SPmartIRL)</t>
+  </si>
+  <si>
+    <t>displayed on the LCD Screen
+Line 1: “SPmart Menu”
+Line 2: “1. Self-Checkout”</t>
+  </si>
+  <si>
+    <t>Run SPmartIRL container</t>
+  </si>
+  <si>
+    <t>Test that pressing "1" starts self checkout process</t>
+  </si>
+  <si>
+    <t>Press "1" on keypad</t>
+  </si>
+  <si>
+    <t>REQ-08 menu shown</t>
+  </si>
+  <si>
+    <t>Test that LCD shows instruction as required</t>
+  </si>
+  <si>
+    <t>Python Container is running (SPmartIRL), "1" Is pressed in main menu</t>
+  </si>
+  <si>
+    <t>Nil (auto runs)</t>
+  </si>
+  <si>
+    <t>displayed on the LCD Screen:
+Line 1: “Scan item”
+Line 2: “at camera”</t>
+  </si>
+  <si>
+    <t>REQ-09-REQ-17</t>
+  </si>
+  <si>
+    <t>Test that Product Scanning works</t>
+  </si>
+  <si>
+    <t>Flowchart in Figure 1 (SRS Doc) is followed</t>
+  </si>
+  <si>
+    <t>Test that Payment Menu shown as required</t>
+  </si>
+  <si>
+    <t>Python Container is running (SPmartIRL), "1" Is pressed in main menu, Products are scanned and user proceeds to payment</t>
+  </si>
+  <si>
+    <t>Press "1" on keypad after scanning products</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Display the following lines on the LCD 
+Line 1: “Payment Method?”
+Line 2: “1. ATM, 2. PayWave”</t>
+  </si>
+  <si>
+    <t>Display the following lines on the LCD 
+Line 1: “Payment Method?”
+Line 2: “1. ATM, 2. PayWave”</t>
+  </si>
+  <si>
+    <t>REQ-19-REQ-35</t>
+  </si>
+  <si>
+    <t>Flowchart in Figure 2 (SRS Doc) is followed</t>
+  </si>
+  <si>
+    <t>REQ-9</t>
+  </si>
+  <si>
+    <t>MySQL Container is running, PyTest Unit Test test_camera_scanning is ran.</t>
+  </si>
+  <si>
+    <t>Point camera at a barcode</t>
+  </si>
+  <si>
+    <t>LCD to display product details fetched from database</t>
+  </si>
+  <si>
+    <t>MySQL Container is running, PyTest Unit Test test_db is ran.</t>
+  </si>
+  <si>
+    <t>Run all tests in test_db.py</t>
+  </si>
+  <si>
+    <t>Run test_verify_pin() in test_main.py</t>
+  </si>
+  <si>
+    <t>Test pass</t>
+  </si>
+  <si>
+    <t>REQ-28-REQ-33</t>
+  </si>
+  <si>
+    <t>Python Container is running, PyTest Unit Test test_pay_with_paywave  is ran.</t>
+  </si>
+  <si>
+    <t>Python Container is running, PyTest Unit Test test_verify_pin() is ran.</t>
+  </si>
+  <si>
+    <t>Test pass, Flowchart steps in Figure 2 REQ-28-33 is followed on RPI Dev Board</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that Payment works</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that Barcode Scanning Works</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that Python is able to fetch data from MySQL databse</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that entering right/wrong PIN works as intended</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that RFID payment (PayWave) is working as intended</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +317,12 @@
       <color rgb="FF333333"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -163,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,11 +386,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -225,18 +436,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -248,13 +456,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -311,7 +512,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -487,13 +687,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,7 +765,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -573,6 +772,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1208,9 +1408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1248,9 +1448,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,7 +1485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1320,7 +1520,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,52 +1693,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+        <f>COUNTIF('Test Cases &amp; Results'!B4:B47, "&lt;&gt;")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Pass")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>19</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Not Tested")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1549,433 +1749,545 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.69140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.15234375" customWidth="1"/>
+    <col min="7" max="7" width="21.69140625" customWidth="1"/>
+    <col min="8" max="8" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.3828125" customWidth="1"/>
+    <col min="10" max="10" width="18.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.53515625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="4" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B5" s="2">
+        <f>B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="44.6" x14ac:dyDescent="0.4">
+      <c r="B6" s="2">
+        <f t="shared" ref="B6:B18" si="0">B5+1</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <f>B3+1</f>
-        <v>2</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B20" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="C7" s="14"/>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="C8" s="14"/>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="C9" s="14"/>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="C10" s="14"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="C11" s="14"/>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="C12" s="14"/>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B14" s="2">
+        <f>B13+1</f>
         <v>11</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="C14" s="14"/>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="C15" s="14"/>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="C16" s="14"/>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="C17" s="14"/>
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="D18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="I18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="K18" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
-        <v>19</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="K4:K18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,17 +2295,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>Enums!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4:K18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Enums!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K22</xm:sqref>
+          <xm:sqref>E6:E7 E1:E2 E4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2002,41 +2314,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Revert "fill in Test Report, update SRS with contributions"
This reverts commit c8e2ea671d84ccde696b605acd1c153e54861293.

revert commit too wrong branch
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD4DFA5-42F4-42FC-9B6F-7578E252B060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -21,8 +20,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -86,217 +83,26 @@
     <t>Low Impact</t>
   </si>
   <si>
-    <t>REQ-06</t>
+    <t>Test that the water heater is activated if the water temperature is &lt; 100 Deg C</t>
   </si>
   <si>
-    <t>REQ-01</t>
+    <t>Water temperature is &lt; 100 Deg C</t>
   </si>
   <si>
-    <t>REQ-02</t>
+    <t>From the LCD main menu, select the option "Black Coffee"</t>
   </si>
   <si>
-    <t>REQ-03</t>
+    <t>-Heating element is activated when water temperature is &lt; 100 Deg C</t>
   </si>
   <si>
-    <t>REQ-04</t>
-  </si>
-  <si>
-    <t>REQ-05</t>
-  </si>
-  <si>
-    <t>REQ-07</t>
-  </si>
-  <si>
-    <t>REQ-08</t>
-  </si>
-  <si>
-    <t>REQ-13</t>
-  </si>
-  <si>
-    <t>REQ-18</t>
-  </si>
-  <si>
-    <t>REQ-23</t>
-  </si>
-  <si>
-    <t>Webserver Container is running (SPmartWeb)</t>
-  </si>
-  <si>
-    <t>Open Localhost/IP Adderess of RPI</t>
-  </si>
-  <si>
-    <t>Products can be seen and added to cart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test that Web Server page shortcuts are shown correctly </t>
-  </si>
-  <si>
-    <t>Test that Web Server pages are shown correctly and content is shown (products)</t>
-  </si>
-  <si>
-    <t>Webserver Container is running (SPmartWeb) Products are added to cart and user is logged in</t>
-  </si>
-  <si>
-    <t>Shortcuts can be seen in Navbar</t>
-  </si>
-  <si>
-    <t>Add a product to cart</t>
-  </si>
-  <si>
-    <t>Test that cart pages functions properly</t>
-  </si>
-  <si>
-    <t>Products are shown in cart and checkout options are shown</t>
-  </si>
-  <si>
-    <t>Test that checkout options works properly</t>
-  </si>
-  <si>
-    <t>Choose a checkout option and checkout</t>
-  </si>
-  <si>
-    <t>Additional price for delivery is shown and added if selected. When checkout, sent to My Orders</t>
-  </si>
-  <si>
-    <t>Test that orders are shown and Self Pickup QR codes are shown</t>
-  </si>
-  <si>
-    <t>Webserver Container is running (SPmartWeb). Order is placed and user is logged in</t>
-  </si>
-  <si>
-    <t>Checkout/Go to My Orders page</t>
-  </si>
-  <si>
-    <t>Orders are shown and QR codes shown where applicable</t>
-  </si>
-  <si>
-    <t>Test that LCD shows menu as required</t>
-  </si>
-  <si>
-    <t>Python Container is running (SPmartIRL)</t>
-  </si>
-  <si>
-    <t>displayed on the LCD Screen
-Line 1: “SPmart Menu”
-Line 2: “1. Self-Checkout”</t>
-  </si>
-  <si>
-    <t>Run SPmartIRL container</t>
-  </si>
-  <si>
-    <t>Test that pressing "1" starts self checkout process</t>
-  </si>
-  <si>
-    <t>Press "1" on keypad</t>
-  </si>
-  <si>
-    <t>REQ-08 menu shown</t>
-  </si>
-  <si>
-    <t>Test that LCD shows instruction as required</t>
-  </si>
-  <si>
-    <t>Python Container is running (SPmartIRL), "1" Is pressed in main menu</t>
-  </si>
-  <si>
-    <t>Nil (auto runs)</t>
-  </si>
-  <si>
-    <t>displayed on the LCD Screen:
-Line 1: “Scan item”
-Line 2: “at camera”</t>
-  </si>
-  <si>
-    <t>REQ-09-REQ-17</t>
-  </si>
-  <si>
-    <t>Test that Product Scanning works</t>
-  </si>
-  <si>
-    <t>Flowchart in Figure 1 (SRS Doc) is followed</t>
-  </si>
-  <si>
-    <t>Test that Payment Menu shown as required</t>
-  </si>
-  <si>
-    <t>Python Container is running (SPmartIRL), "1" Is pressed in main menu, Products are scanned and user proceeds to payment</t>
-  </si>
-  <si>
-    <t>Press "1" on keypad after scanning products</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Display the following lines on the LCD 
-Line 1: “Payment Method?”
-Line 2: “1. ATM, 2. PayWave”</t>
-  </si>
-  <si>
-    <t>Display the following lines on the LCD 
-Line 1: “Payment Method?”
-Line 2: “1. ATM, 2. PayWave”</t>
-  </si>
-  <si>
-    <t>REQ-19-REQ-35</t>
-  </si>
-  <si>
-    <t>Flowchart in Figure 2 (SRS Doc) is followed</t>
-  </si>
-  <si>
-    <t>REQ-9</t>
-  </si>
-  <si>
-    <t>MySQL Container is running, PyTest Unit Test test_camera_scanning is ran.</t>
-  </si>
-  <si>
-    <t>Point camera at a barcode</t>
-  </si>
-  <si>
-    <t>LCD to display product details fetched from database</t>
-  </si>
-  <si>
-    <t>MySQL Container is running, PyTest Unit Test test_db is ran.</t>
-  </si>
-  <si>
-    <t>Run all tests in test_db.py</t>
-  </si>
-  <si>
-    <t>Run test_verify_pin() in test_main.py</t>
-  </si>
-  <si>
-    <t>Test pass</t>
-  </si>
-  <si>
-    <t>REQ-28-REQ-33</t>
-  </si>
-  <si>
-    <t>Python Container is running, PyTest Unit Test test_pay_with_paywave  is ran.</t>
-  </si>
-  <si>
-    <t>Python Container is running, PyTest Unit Test test_verify_pin() is ran.</t>
-  </si>
-  <si>
-    <t>Test pass, Flowchart steps in Figure 2 REQ-28-33 is followed on RPI Dev Board</t>
-  </si>
-  <si>
-    <t>(PyTest) Test that Payment works</t>
-  </si>
-  <si>
-    <t>(PyTest) Test that Barcode Scanning Works</t>
-  </si>
-  <si>
-    <t>(PyTest) Test that Python is able to fetch data from MySQL databse</t>
-  </si>
-  <si>
-    <t>(PyTest) Test that entering right/wrong PIN works as intended</t>
-  </si>
-  <si>
-    <t>(PyTest) Test that RFID payment (PayWave) is working as intended</t>
+    <t>REQ-06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,12 +123,6 @@
       <color rgb="FF333333"/>
       <name val="Verdana"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -363,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -386,22 +186,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -436,15 +225,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -456,6 +248,13 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -512,6 +311,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -687,13 +487,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -765,6 +565,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -772,7 +573,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1408,9 +1208,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1448,9 +1248,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1485,7 +1285,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1520,7 +1320,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1693,52 +1493,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="129" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!B4:B47, "&lt;&gt;")</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+        <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Pass")</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Fail")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Not Tested")</f>
-        <v>0</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1749,545 +1549,433 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:K18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.15234375" customWidth="1"/>
-    <col min="7" max="7" width="21.69140625" customWidth="1"/>
-    <col min="8" max="8" width="25.3046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.3828125" customWidth="1"/>
-    <col min="10" max="10" width="18.53515625" customWidth="1"/>
-    <col min="11" max="11" width="12.53515625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-    </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B3" s="1" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>31</v>
-      </c>
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <f>B4+1</f>
-        <v>2</v>
+        <f t="shared" ref="B5:B20" si="0">B4+1</f>
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>35</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="44.6" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
-        <f t="shared" ref="B6:B18" si="0">B5+1</f>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="14"/>
-      <c r="D7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>41</v>
-      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="14"/>
-      <c r="D8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>45</v>
-      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="87.45" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>48</v>
-      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>52</v>
-      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="58.3" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="14"/>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>56</v>
-      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="14"/>
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>59</v>
-      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
       <c r="K12" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="87.45" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="14"/>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>64</v>
-      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
       <c r="K13" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <f>B13+1</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="C14" s="14"/>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>61</v>
-      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>66</v>
-      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
       <c r="K14" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C15" s="14"/>
-      <c r="D15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>70</v>
-      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
       <c r="K15" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" s="14"/>
-      <c r="D16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>70</v>
-      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="14"/>
-      <c r="D17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>74</v>
-      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>76</v>
-      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>78</v>
-      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="12" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <f t="shared" ref="B21:B22" si="1">B20+1</f>
+        <v>19</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="12" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="K4:K18">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="K3:K20">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K20">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:K22">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21:K22">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2295,17 +1983,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Enums!$B$8:$B$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K4:K18</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
-            <xm:f>Enums!$B$8:$B$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>E6:E7 E1:E2 E4</xm:sqref>
+          <xm:sqref>K3:K22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2314,41 +2002,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
fill in test report, update SRS doc with contribution
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD4DFA5-42F4-42FC-9B6F-7578E252B060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -83,26 +86,217 @@
     <t>Low Impact</t>
   </si>
   <si>
-    <t>Test that the water heater is activated if the water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>Water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
-    <t>From the LCD main menu, select the option "Black Coffee"</t>
-  </si>
-  <si>
-    <t>-Heating element is activated when water temperature is &lt; 100 Deg C</t>
-  </si>
-  <si>
     <t>REQ-06</t>
+  </si>
+  <si>
+    <t>REQ-01</t>
+  </si>
+  <si>
+    <t>REQ-02</t>
+  </si>
+  <si>
+    <t>REQ-03</t>
+  </si>
+  <si>
+    <t>REQ-04</t>
+  </si>
+  <si>
+    <t>REQ-05</t>
+  </si>
+  <si>
+    <t>REQ-07</t>
+  </si>
+  <si>
+    <t>REQ-08</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>REQ-18</t>
+  </si>
+  <si>
+    <t>REQ-23</t>
+  </si>
+  <si>
+    <t>Webserver Container is running (SPmartWeb)</t>
+  </si>
+  <si>
+    <t>Open Localhost/IP Adderess of RPI</t>
+  </si>
+  <si>
+    <t>Products can be seen and added to cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that Web Server page shortcuts are shown correctly </t>
+  </si>
+  <si>
+    <t>Test that Web Server pages are shown correctly and content is shown (products)</t>
+  </si>
+  <si>
+    <t>Webserver Container is running (SPmartWeb) Products are added to cart and user is logged in</t>
+  </si>
+  <si>
+    <t>Shortcuts can be seen in Navbar</t>
+  </si>
+  <si>
+    <t>Add a product to cart</t>
+  </si>
+  <si>
+    <t>Test that cart pages functions properly</t>
+  </si>
+  <si>
+    <t>Products are shown in cart and checkout options are shown</t>
+  </si>
+  <si>
+    <t>Test that checkout options works properly</t>
+  </si>
+  <si>
+    <t>Choose a checkout option and checkout</t>
+  </si>
+  <si>
+    <t>Additional price for delivery is shown and added if selected. When checkout, sent to My Orders</t>
+  </si>
+  <si>
+    <t>Test that orders are shown and Self Pickup QR codes are shown</t>
+  </si>
+  <si>
+    <t>Webserver Container is running (SPmartWeb). Order is placed and user is logged in</t>
+  </si>
+  <si>
+    <t>Checkout/Go to My Orders page</t>
+  </si>
+  <si>
+    <t>Orders are shown and QR codes shown where applicable</t>
+  </si>
+  <si>
+    <t>Test that LCD shows menu as required</t>
+  </si>
+  <si>
+    <t>Python Container is running (SPmartIRL)</t>
+  </si>
+  <si>
+    <t>displayed on the LCD Screen
+Line 1: “SPmart Menu”
+Line 2: “1. Self-Checkout”</t>
+  </si>
+  <si>
+    <t>Run SPmartIRL container</t>
+  </si>
+  <si>
+    <t>Test that pressing "1" starts self checkout process</t>
+  </si>
+  <si>
+    <t>Press "1" on keypad</t>
+  </si>
+  <si>
+    <t>REQ-08 menu shown</t>
+  </si>
+  <si>
+    <t>Test that LCD shows instruction as required</t>
+  </si>
+  <si>
+    <t>Python Container is running (SPmartIRL), "1" Is pressed in main menu</t>
+  </si>
+  <si>
+    <t>Nil (auto runs)</t>
+  </si>
+  <si>
+    <t>displayed on the LCD Screen:
+Line 1: “Scan item”
+Line 2: “at camera”</t>
+  </si>
+  <si>
+    <t>REQ-09-REQ-17</t>
+  </si>
+  <si>
+    <t>Test that Product Scanning works</t>
+  </si>
+  <si>
+    <t>Flowchart in Figure 1 (SRS Doc) is followed</t>
+  </si>
+  <si>
+    <t>Test that Payment Menu shown as required</t>
+  </si>
+  <si>
+    <t>Python Container is running (SPmartIRL), "1" Is pressed in main menu, Products are scanned and user proceeds to payment</t>
+  </si>
+  <si>
+    <t>Press "1" on keypad after scanning products</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Display the following lines on the LCD 
+Line 1: “Payment Method?”
+Line 2: “1. ATM, 2. PayWave”</t>
+  </si>
+  <si>
+    <t>Display the following lines on the LCD 
+Line 1: “Payment Method?”
+Line 2: “1. ATM, 2. PayWave”</t>
+  </si>
+  <si>
+    <t>REQ-19-REQ-35</t>
+  </si>
+  <si>
+    <t>Flowchart in Figure 2 (SRS Doc) is followed</t>
+  </si>
+  <si>
+    <t>REQ-9</t>
+  </si>
+  <si>
+    <t>MySQL Container is running, PyTest Unit Test test_camera_scanning is ran.</t>
+  </si>
+  <si>
+    <t>Point camera at a barcode</t>
+  </si>
+  <si>
+    <t>LCD to display product details fetched from database</t>
+  </si>
+  <si>
+    <t>MySQL Container is running, PyTest Unit Test test_db is ran.</t>
+  </si>
+  <si>
+    <t>Run all tests in test_db.py</t>
+  </si>
+  <si>
+    <t>Run test_verify_pin() in test_main.py</t>
+  </si>
+  <si>
+    <t>Test pass</t>
+  </si>
+  <si>
+    <t>REQ-28-REQ-33</t>
+  </si>
+  <si>
+    <t>Python Container is running, PyTest Unit Test test_pay_with_paywave  is ran.</t>
+  </si>
+  <si>
+    <t>Python Container is running, PyTest Unit Test test_verify_pin() is ran.</t>
+  </si>
+  <si>
+    <t>Test pass, Flowchart steps in Figure 2 REQ-28-33 is followed on RPI Dev Board</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that Payment works</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that Barcode Scanning Works</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that Python is able to fetch data from MySQL databse</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that entering right/wrong PIN works as intended</t>
+  </si>
+  <si>
+    <t>(PyTest) Test that RFID payment (PayWave) is working as intended</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +317,12 @@
       <color rgb="FF333333"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -163,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -186,11 +386,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -225,18 +436,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -248,13 +456,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -311,7 +512,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -487,13 +687,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,7 +765,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -573,6 +772,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1208,9 +1408,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1248,9 +1448,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,7 +1485,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1320,7 +1520,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,52 +1693,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
-    <sheetView zoomScale="129" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+        <f>COUNTIF('Test Cases &amp; Results'!B4:B47, "&lt;&gt;")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Pass")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="10">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>19</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K4:K49, "Not Tested")</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1549,433 +1749,545 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.69140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.15234375" customWidth="1"/>
+    <col min="7" max="7" width="21.69140625" customWidth="1"/>
+    <col min="8" max="8" width="25.3046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.3828125" customWidth="1"/>
+    <col min="10" max="10" width="18.53515625" customWidth="1"/>
+    <col min="11" max="11" width="12.53515625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="4" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B5" s="2">
+        <f>B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="44.6" x14ac:dyDescent="0.4">
+      <c r="B6" s="2">
+        <f t="shared" ref="B6:B18" si="0">B5+1</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="12" t="s">
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <f>B3+1</f>
-        <v>2</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <f t="shared" ref="B5:B20" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="C7" s="14"/>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="C8" s="14"/>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="C9" s="14"/>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="C10" s="14"/>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="C11" s="14"/>
+      <c r="D11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="C12" s="14"/>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="87.45" x14ac:dyDescent="0.4">
+      <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B14" s="2">
+        <f>B13+1</f>
         <v>11</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="C14" s="14"/>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="C15" s="14"/>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="C16" s="14"/>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="C17" s="14"/>
+      <c r="D17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
       <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="D18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>76</v>
+      </c>
       <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="I18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="K18" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
-        <v>19</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="K4:K18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,17 +2295,17 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>Enums!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4:K18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E5</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Enums!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>K3:K22</xm:sqref>
+          <xm:sqref>E6:E7 E1:E2 E4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2002,41 +2314,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3828125" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>17</v>
       </c>

</xml_diff>